<commit_message>
new changes to docs and code
</commit_message>
<xml_diff>
--- a/data/requet_notesT.xlsx
+++ b/data/requet_notesT.xlsx
@@ -2775,7 +2775,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2789,6 +2789,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2798,7 +2804,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -2827,13 +2840,13 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -3157,13 +3170,13 @@
     <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -3171,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -3179,7 +3192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3187,7 +3200,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3195,7 +3208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3203,7 +3216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3211,7 +3224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3219,7 +3232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3227,7 +3240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3235,7 +3248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3243,7 +3256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>11</v>
       </c>

</xml_diff>